<commit_message>
update quick registration for employer
</commit_message>
<xml_diff>
--- a/HPA/brand.xlsx
+++ b/HPA/brand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15210" windowHeight="6405"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Shee1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>BrandName</t>
   </si>
@@ -40,20 +40,49 @@
     <t>Media</t>
   </si>
   <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>ada</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>hello brand</t>
+  </si>
+  <si>
+    <t>Redline tuning</t>
+  </si>
+  <si>
+    <t>Ha-Banai Street 29, Holon, 58857, Israel</t>
+  </si>
+  <si>
+    <t>Event/Catering</t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>HarriTest</t>
+  </si>
+  <si>
+    <t>C:\\Users\\Harri\\Desktop\\Food.jpg</t>
+  </si>
+  <si>
+    <t>test@harri.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -76,13 +105,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,7 +417,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,28 +458,34 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1231231</v>
-      </c>
-      <c r="B2">
-        <v>12312</v>
-      </c>
-      <c r="C2">
-        <v>1231</v>
-      </c>
-      <c r="D2">
-        <v>123123</v>
-      </c>
-      <c r="E2">
-        <v>1231213</v>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25"/>
@@ -457,6 +495,9 @@
     <row r="7" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update employer quick registration
</commit_message>
<xml_diff>
--- a/HPA/brand.xlsx
+++ b/HPA/brand.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="6405"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14790" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Shee1" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
     <t>Redline tuning</t>
   </si>
   <si>
-    <t>Ha-Banai Street 29, Holon, 58857, Israel</t>
-  </si>
-  <si>
     <t>Event/Catering</t>
   </si>
   <si>
@@ -61,10 +58,13 @@
     <t>HarriTest</t>
   </si>
   <si>
-    <t>C:\\Users\\Harri\\Desktop\\Food.jpg</t>
-  </si>
-  <si>
     <t>test@harri.com</t>
+  </si>
+  <si>
+    <t>Ha-Banai St 29, Holon, 58857, Israel</t>
+  </si>
+  <si>
+    <t>C:\Users\Harri\Desktop\Food.jpg||,</t>
   </si>
 </sst>
 </file>
@@ -416,19 +416,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="53.140625" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="10" max="10" width="17.5703125" customWidth="1"/>
@@ -467,22 +467,22 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>

</xml_diff>